<commit_message>
Weekly Status Report updated
</commit_message>
<xml_diff>
--- a/HTD Programs-Weekly Status Report for Capgemini.xlsx
+++ b/HTD Programs-Weekly Status Report for Capgemini.xlsx
@@ -2297,9 +2297,6 @@
     <t>Reviewed-Project Going On</t>
   </si>
   <si>
-    <t>Reviewed-Ready for Test</t>
-  </si>
-  <si>
     <t>Parallel Project Name</t>
   </si>
   <si>
@@ -2353,16 +2350,20 @@
     <t>Varsha has reviewd M1 MTT &amp; MPT on Thrusday 17th Oct 2019</t>
   </si>
   <si>
-    <t>BDD is Completed
-Module 4 Test Conducted</t>
-  </si>
-  <si>
-    <t>Core Java, SQL and JDBC Completed
-Module 1 Test Conducted</t>
-  </si>
-  <si>
-    <t>Core Java is going on
-SQL Completed</t>
+    <t>Parllel Project Evalution Done
+PLP Started</t>
+  </si>
+  <si>
+    <t>HTML5, CSS3 with bootstrap 4 completed
+Javascript and Typescript completed
+Angular Started</t>
+  </si>
+  <si>
+    <t>Core Java and Sql completed
+JDBC going on</t>
+  </si>
+  <si>
+    <t>Project Evaluated</t>
   </si>
 </sst>
 </file>
@@ -4272,10 +4273,10 @@
   <dimension ref="B2:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +4355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4401,14 +4402,14 @@
         <v>9448246364</v>
       </c>
       <c r="P3" s="59" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="2:18" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -4439,11 +4440,11 @@
       </c>
       <c r="K4" s="36">
         <f>'Noida Batch Candidates'!D3</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L4" s="34">
         <f>'Noida Batch Candidates'!D4</f>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>11</v>
@@ -4455,14 +4456,14 @@
         <v>8377841525</v>
       </c>
       <c r="P4" s="60" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="2:18" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -4509,14 +4510,14 @@
         <v>8073098283</v>
       </c>
       <c r="P5" s="60" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>15</v>
       </c>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="2:18" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -4547,11 +4548,11 @@
       </c>
       <c r="K6" s="36">
         <f>'Bangalore Batch Candidates'!D3</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L6" s="34">
         <f>'Bangalore Batch Candidates'!D4</f>
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>13</v>
@@ -4563,14 +4564,14 @@
         <v>8762928822</v>
       </c>
       <c r="P6" s="60" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>15</v>
       </c>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="2:18" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -4601,11 +4602,11 @@
       </c>
       <c r="K7" s="36">
         <f>'Pune-Mumbai Batch Candidates'!D3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L7" s="34">
         <f>'Pune-Mumbai Batch Candidates'!D4</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>14</v>
@@ -4617,7 +4618,7 @@
         <v>9897145195</v>
       </c>
       <c r="P7" s="60" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -4654,8 +4655,7 @@
     <col min="6" max="7" width="45.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="39" style="24" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="45.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="33.5703125" style="24" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="32.140625" style="54" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="34.140625" style="54" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="42.7109375" style="51" bestFit="1" customWidth="1"/>
@@ -4664,13 +4664,13 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="61" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
       <c r="F2" s="62" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G2" s="62"/>
       <c r="H2" s="58"/>
@@ -4716,13 +4716,13 @@
         <v>753</v>
       </c>
       <c r="P4" s="66" t="s">
+        <v>758</v>
+      </c>
+      <c r="Q4" s="66" t="s">
         <v>759</v>
       </c>
-      <c r="Q4" s="66" t="s">
-        <v>760</v>
-      </c>
       <c r="R4" s="66" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="5" spans="2:18" s="31" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4796,25 +4796,25 @@
         <v>755</v>
       </c>
       <c r="L6" s="41" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="M6" s="41" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="N6" s="41" t="s">
+        <v>778</v>
+      </c>
+      <c r="O6" s="41" t="s">
         <v>757</v>
       </c>
-      <c r="O6" s="41" t="s">
-        <v>758</v>
-      </c>
       <c r="P6" s="53" t="s">
+        <v>760</v>
+      </c>
+      <c r="Q6" s="53" t="s">
         <v>761</v>
       </c>
-      <c r="Q6" s="53" t="s">
-        <v>762</v>
-      </c>
       <c r="R6" s="52" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
@@ -4865,13 +4865,13 @@
         <v>754</v>
       </c>
       <c r="P7" s="53" t="s">
+        <v>768</v>
+      </c>
+      <c r="Q7" s="53" t="s">
         <v>769</v>
       </c>
-      <c r="Q7" s="53" t="s">
-        <v>770</v>
-      </c>
       <c r="R7" s="63" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
@@ -4922,10 +4922,10 @@
         <v>754</v>
       </c>
       <c r="P8" s="53" t="s">
+        <v>765</v>
+      </c>
+      <c r="Q8" s="53" t="s">
         <v>766</v>
-      </c>
-      <c r="Q8" s="53" t="s">
-        <v>767</v>
       </c>
       <c r="R8" s="64"/>
     </row>
@@ -4977,10 +4977,10 @@
         <v>754</v>
       </c>
       <c r="P9" s="53" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="Q9" s="53" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="R9" s="65"/>
     </row>
@@ -5002,10 +5002,10 @@
         <v>Sudheer</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="H10" s="41" t="s">
         <v>754</v>
@@ -5032,10 +5032,10 @@
         <v>754</v>
       </c>
       <c r="P10" s="53" t="s">
+        <v>770</v>
+      </c>
+      <c r="Q10" s="53" t="s">
         <v>771</v>
-      </c>
-      <c r="Q10" s="53" t="s">
-        <v>772</v>
       </c>
       <c r="R10" s="52"/>
     </row>
@@ -6441,7 +6441,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L34"/>
+  <dimension ref="B2:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="D3" s="22">
         <f>COUNT($H$1:$H$100)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -6489,7 +6489,7 @@
       </c>
       <c r="D4" s="22">
         <f>COUNT($B$1:$B$100)</f>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -6734,16 +6734,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="27">
-        <v>9368519717</v>
+        <v>8512097276</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="H14" s="33">
         <v>7</v>
@@ -6766,16 +6766,16 @@
         <v>8</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="27">
-        <v>8115712543</v>
+        <v>8076728958</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="H15" s="33">
         <v>8</v>
@@ -6798,16 +6798,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="27">
-        <v>8512097276</v>
+        <v>7669604203</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="H16" s="33">
         <v>9</v>
@@ -6830,16 +6830,16 @@
         <v>10</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E17" s="27">
-        <v>8076728958</v>
+        <v>8860817681</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="H17" s="33">
         <v>10</v>
@@ -6862,16 +6862,16 @@
         <v>11</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="27">
-        <v>7669604203</v>
+        <v>9015270530</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="H18" s="33">
         <v>11</v>
@@ -6894,16 +6894,16 @@
         <v>12</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E19" s="27">
-        <v>8860817681</v>
+        <v>7827327267</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="H19" s="33">
         <v>12</v>
@@ -6926,16 +6926,16 @@
         <v>13</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="27">
-        <v>9015270530</v>
+        <v>8800709136</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="H20" s="33">
         <v>13</v>
@@ -6958,16 +6958,16 @@
         <v>14</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E21" s="27">
-        <v>7827327267</v>
+        <v>9971884734</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="H21" s="33">
         <v>14</v>
@@ -6990,16 +6990,16 @@
         <v>15</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E22" s="27">
-        <v>8800709136</v>
+        <v>7988643977</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="H22" s="33">
         <v>15</v>
@@ -7022,16 +7022,16 @@
         <v>16</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E23" s="27">
-        <v>9971884734</v>
+        <v>9910920931</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H23" s="33">
         <v>16</v>
@@ -7054,16 +7054,16 @@
         <v>17</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E24" s="27">
-        <v>7988643977</v>
+        <v>7073862831</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="H24" s="33">
         <v>17</v>
@@ -7086,16 +7086,16 @@
         <v>18</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E25" s="27">
-        <v>9910920931</v>
+        <v>9810943877</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="H25" s="33">
         <v>18</v>
@@ -7118,16 +7118,16 @@
         <v>19</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E26" s="27">
-        <v>7073862831</v>
+        <v>9582848409</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="H26" s="33">
         <v>19</v>
@@ -7150,16 +7150,16 @@
         <v>20</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="27">
-        <v>9810943877</v>
+        <v>7065509255</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="H27" s="33">
         <v>20</v>
@@ -7182,16 +7182,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E28" s="27">
-        <v>9582848409</v>
+        <v>8218128166</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="H28" s="33">
         <v>21</v>
@@ -7214,16 +7214,16 @@
         <v>22</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E29" s="27">
-        <v>7065509255</v>
+        <v>8512856779</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="H29" s="33">
         <v>22</v>
@@ -7246,16 +7246,16 @@
         <v>23</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="27">
-        <v>9897133664</v>
+        <v>9067472225</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="H30" s="33">
         <v>23</v>
@@ -7274,21 +7274,6 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="32">
-        <v>24</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>537</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="27">
-        <v>8218128166</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>538</v>
-      </c>
       <c r="H31" s="33">
         <v>24</v>
       </c>
@@ -7306,21 +7291,6 @@
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="32">
-        <v>25</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>539</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="27">
-        <v>8512856779</v>
-      </c>
-      <c r="F32" s="25" t="s">
-        <v>540</v>
-      </c>
       <c r="H32" s="33">
         <v>25</v>
       </c>
@@ -7337,37 +7307,71 @@
         <v>618</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="32">
+    <row r="33" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H33" s="32">
         <v>26</v>
       </c>
-      <c r="C33" s="25" t="s">
-        <v>541</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="27">
-        <v>9067472225</v>
-      </c>
-      <c r="F33" s="25" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="32">
+      <c r="I33" s="25" t="s">
+        <v>503</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K33" s="27">
+        <v>9368519717</v>
+      </c>
+      <c r="L33" s="25" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="34" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H34" s="32">
         <v>27</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="I34" s="25" t="s">
+        <v>505</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K34" s="27">
+        <v>8115712543</v>
+      </c>
+      <c r="L34" s="25" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="35" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H35" s="32">
+        <v>28</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>535</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K35" s="27">
+        <v>9897133664</v>
+      </c>
+      <c r="L35" s="25" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="36" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H36" s="32">
+        <v>29</v>
+      </c>
+      <c r="I36" s="25" t="s">
         <v>543</v>
       </c>
-      <c r="D34" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="27">
+      <c r="J36" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K36" s="27">
         <v>8604793053</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="L36" s="25" t="s">
         <v>544</v>
       </c>
     </row>
@@ -7377,32 +7381,32 @@
     <mergeCell ref="H6:I6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F21" r:id="rId1"/>
-    <hyperlink ref="F23" r:id="rId2"/>
-    <hyperlink ref="F15" r:id="rId3"/>
+    <hyperlink ref="F19" r:id="rId1"/>
+    <hyperlink ref="F21" r:id="rId2"/>
+    <hyperlink ref="L34" r:id="rId3"/>
     <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F14" r:id="rId5"/>
-    <hyperlink ref="F26" r:id="rId6"/>
-    <hyperlink ref="F19" r:id="rId7"/>
+    <hyperlink ref="L33" r:id="rId5"/>
+    <hyperlink ref="F24" r:id="rId6"/>
+    <hyperlink ref="F17" r:id="rId7"/>
     <hyperlink ref="F11" r:id="rId8"/>
     <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="F17" r:id="rId10"/>
-    <hyperlink ref="F16" r:id="rId11"/>
-    <hyperlink ref="F25" r:id="rId12"/>
+    <hyperlink ref="F15" r:id="rId10"/>
+    <hyperlink ref="F14" r:id="rId11"/>
+    <hyperlink ref="F23" r:id="rId12"/>
     <hyperlink ref="F10" r:id="rId13"/>
-    <hyperlink ref="F32" r:id="rId14"/>
-    <hyperlink ref="F29" r:id="rId15"/>
-    <hyperlink ref="F24" r:id="rId16"/>
-    <hyperlink ref="F20" r:id="rId17"/>
-    <hyperlink ref="F18" r:id="rId18"/>
-    <hyperlink ref="F28" r:id="rId19"/>
-    <hyperlink ref="F22" r:id="rId20"/>
+    <hyperlink ref="F29" r:id="rId14"/>
+    <hyperlink ref="F27" r:id="rId15"/>
+    <hyperlink ref="F22" r:id="rId16"/>
+    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F16" r:id="rId18"/>
+    <hyperlink ref="F26" r:id="rId19"/>
+    <hyperlink ref="F20" r:id="rId20"/>
     <hyperlink ref="F13" r:id="rId21"/>
     <hyperlink ref="F12" r:id="rId22"/>
-    <hyperlink ref="F30" r:id="rId23"/>
-    <hyperlink ref="F34" r:id="rId24"/>
-    <hyperlink ref="F33" r:id="rId25"/>
-    <hyperlink ref="F31" r:id="rId26"/>
+    <hyperlink ref="L35" r:id="rId23"/>
+    <hyperlink ref="L36" r:id="rId24"/>
+    <hyperlink ref="F30" r:id="rId25"/>
+    <hyperlink ref="F28" r:id="rId26"/>
     <hyperlink ref="L32" r:id="rId27" display="mailto:vishal2897@gmail.com"/>
     <hyperlink ref="L31" r:id="rId28" display="mailto:vinay2135@gmail.com"/>
     <hyperlink ref="L30" r:id="rId29" display="mailto:surbhisangal1997@gmail.com"/>
@@ -7764,7 +7768,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L79"/>
+  <dimension ref="B1:L74"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7809,7 +7813,7 @@
       </c>
       <c r="D3" s="22">
         <f>COUNT($H$1:$H$100)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H3" s="31"/>
     </row>
@@ -7821,7 +7825,7 @@
       </c>
       <c r="D4" s="22">
         <f>COUNT($B$1:$B$100)</f>
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H4" s="31"/>
     </row>
@@ -7877,16 +7881,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
@@ -7909,16 +7913,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H9" s="3">
         <v>2</v>
@@ -7941,16 +7945,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H10" s="3">
         <v>3</v>
@@ -7973,16 +7977,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="H11" s="3">
         <v>4</v>
@@ -8005,16 +8009,16 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="H12" s="3">
         <v>5</v>
@@ -8037,16 +8041,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="H13" s="3">
         <v>6</v>
@@ -8069,16 +8073,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="H14" s="3">
         <v>7</v>
@@ -8101,16 +8105,16 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="H15" s="3">
         <v>8</v>
@@ -8133,16 +8137,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="H16" s="3">
         <v>9</v>
@@ -8165,16 +8169,16 @@
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="H17" s="3">
         <v>10</v>
@@ -8197,16 +8201,31 @@
         <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>274</v>
+        <v>283</v>
+      </c>
+      <c r="H18" s="3">
+        <v>11</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -8214,16 +8233,31 @@
         <v>12</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>277</v>
+        <v>286</v>
+      </c>
+      <c r="H19" s="3">
+        <v>12</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
@@ -8231,16 +8265,31 @@
         <v>13</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>280</v>
+        <v>289</v>
+      </c>
+      <c r="H20" s="3">
+        <v>13</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
@@ -8248,16 +8297,31 @@
         <v>14</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>283</v>
+        <v>292</v>
+      </c>
+      <c r="H21" s="3">
+        <v>14</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -8265,16 +8329,31 @@
         <v>15</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>286</v>
+        <v>295</v>
+      </c>
+      <c r="H22" s="3">
+        <v>15</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
@@ -8282,16 +8361,16 @@
         <v>16</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
@@ -8299,16 +8378,16 @@
         <v>17</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
@@ -8316,16 +8395,16 @@
         <v>18</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
@@ -8333,16 +8412,16 @@
         <v>19</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -8350,16 +8429,16 @@
         <v>20</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -8367,16 +8446,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
@@ -8384,16 +8463,16 @@
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -8401,16 +8480,16 @@
         <v>23</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
@@ -8418,16 +8497,16 @@
         <v>24</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -8435,16 +8514,16 @@
         <v>25</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -8452,16 +8531,16 @@
         <v>26</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -8469,16 +8548,16 @@
         <v>27</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -8486,16 +8565,16 @@
         <v>28</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -8503,16 +8582,16 @@
         <v>29</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -8520,16 +8599,16 @@
         <v>30</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -8537,16 +8616,16 @@
         <v>31</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -8554,16 +8633,16 @@
         <v>32</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -8571,16 +8650,16 @@
         <v>33</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -8588,16 +8667,16 @@
         <v>34</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -8605,16 +8684,16 @@
         <v>35</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -8622,16 +8701,16 @@
         <v>36</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -8639,16 +8718,16 @@
         <v>37</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -8656,16 +8735,16 @@
         <v>38</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -8673,16 +8752,16 @@
         <v>39</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -8690,16 +8769,16 @@
         <v>40</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -8707,16 +8786,16 @@
         <v>41</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -8724,16 +8803,16 @@
         <v>42</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -8741,16 +8820,16 @@
         <v>43</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -8758,16 +8837,16 @@
         <v>44</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -8775,16 +8854,16 @@
         <v>45</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
@@ -8792,16 +8871,16 @@
         <v>46</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
@@ -8809,16 +8888,16 @@
         <v>47</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
@@ -8826,16 +8905,16 @@
         <v>48</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -8843,16 +8922,16 @@
         <v>49</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
@@ -8860,16 +8939,16 @@
         <v>50</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -8877,16 +8956,16 @@
         <v>51</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
@@ -8894,16 +8973,16 @@
         <v>52</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -8911,16 +8990,16 @@
         <v>53</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
@@ -8928,16 +9007,16 @@
         <v>54</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -8945,16 +9024,16 @@
         <v>55</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
@@ -8962,16 +9041,16 @@
         <v>56</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
@@ -8979,16 +9058,16 @@
         <v>57</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
@@ -8996,16 +9075,16 @@
         <v>58</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
@@ -9013,16 +9092,16 @@
         <v>59</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
@@ -9030,16 +9109,16 @@
         <v>60</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
@@ -9047,16 +9126,16 @@
         <v>61</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
@@ -9064,16 +9143,16 @@
         <v>62</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
@@ -9081,16 +9160,16 @@
         <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
@@ -9098,16 +9177,16 @@
         <v>64</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>431</v>
+        <v>446</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>433</v>
+        <v>448</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
@@ -9115,16 +9194,16 @@
         <v>65</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>434</v>
+        <v>449</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>436</v>
+        <v>451</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
@@ -9132,16 +9211,16 @@
         <v>66</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>437</v>
+        <v>452</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>438</v>
+        <v>453</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>439</v>
+        <v>454</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
@@ -9149,100 +9228,15 @@
         <v>67</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>440</v>
+        <v>455</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="3">
-        <v>68</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="3">
-        <v>69</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="3">
-        <v>70</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="3">
-        <v>71</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="3">
-        <v>72</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="F79" s="17" t="s">
         <v>457</v>
       </c>
     </row>
@@ -9252,78 +9246,78 @@
     <mergeCell ref="H6:I6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="mailto:kalyani.addagada@gmail.com"/>
-    <hyperlink ref="F9" r:id="rId2" display="mailto:amulyaps18@gmail.com"/>
-    <hyperlink ref="F10" r:id="rId3" display="mailto:tanilkumarreddy1998@gmail.com"/>
-    <hyperlink ref="F11" r:id="rId4" display="mailto:anjanashaju1997@gmail.com"/>
-    <hyperlink ref="F12" r:id="rId5" display="mailto:aartipawar070@gmail.com"/>
-    <hyperlink ref="F13" r:id="rId6" display="mailto:akbiswal0108@gmail.com"/>
-    <hyperlink ref="F14" r:id="rId7" display="mailto:hiregoudarpita777@gmail.com"/>
-    <hyperlink ref="F15" r:id="rId8" display="mailto:ashalr1997@gmail.com"/>
-    <hyperlink ref="F16" r:id="rId9" display="mailto:bhavyasree.banyala28@gmail.com"/>
-    <hyperlink ref="F17" r:id="rId10" display="mailto:basavarajtoli1800@gmail.com"/>
-    <hyperlink ref="F18" r:id="rId11" display="mailto:bhagyashree.preety321@gmail.com"/>
-    <hyperlink ref="F19" r:id="rId12" display="mailto:bharathachar437@gmail.com"/>
-    <hyperlink ref="F20" r:id="rId13" display="mailto:bhoomika.n89@gmail.com"/>
-    <hyperlink ref="F21" r:id="rId14" display="mailto:patisagar.1997@gmail.com"/>
-    <hyperlink ref="F22" r:id="rId15" display="mailto:chandulokesh426@gmail.com"/>
-    <hyperlink ref="F23" r:id="rId16" display="mailto:jaggu8191@gmail.com"/>
-    <hyperlink ref="F24" r:id="rId17" display="mailto:tejudesireddy4@gmail.com"/>
-    <hyperlink ref="F25" r:id="rId18" display="mailto:g.pavankalyan1998@gmail.com"/>
-    <hyperlink ref="F26" r:id="rId19" display="mailto:gayathrigayigk18@gmail.com"/>
-    <hyperlink ref="F27" r:id="rId20" display="mailto:yasasvi98@gmail.com"/>
-    <hyperlink ref="F28" r:id="rId21" display="mailto:reshueee.rymec@gmail.com"/>
-    <hyperlink ref="F29" r:id="rId22" display="mailto:kajalsinghmys@gmail.com"/>
-    <hyperlink ref="F30" r:id="rId23" display="mailto:skeerti00@gmail.com"/>
-    <hyperlink ref="F31" r:id="rId24" display="mailto:khadirshaik722@gmail.com"/>
-    <hyperlink ref="F32" r:id="rId25" display="mailto:guna.konda333@gmail.com"/>
-    <hyperlink ref="F33" r:id="rId26" display="mailto:mvmkoushik@gmail.com"/>
-    <hyperlink ref="F34" r:id="rId27" display="mailto:maluguveluanusha@gmail.com"/>
-    <hyperlink ref="F35" r:id="rId28" display="mailto:chundurumahendra@gmail.com"/>
-    <hyperlink ref="F36" r:id="rId29" display="mailto:hussainsaddan786@gmail.com"/>
-    <hyperlink ref="F37" r:id="rId30" display="mailto:vasuda.mikkilineni@gmail.com"/>
-    <hyperlink ref="F38" r:id="rId31" display="mailto:sureshma.reddy1997@gmail.com"/>
-    <hyperlink ref="F39" r:id="rId32" display="mailto:pallavi.nelli1@gmail.com"/>
-    <hyperlink ref="F40" r:id="rId33" display="mailto:mounikasharan4321@gmail.com"/>
-    <hyperlink ref="F41" r:id="rId34" display="mailto:venkatasaiprasad99@gmail.com"/>
-    <hyperlink ref="F42" r:id="rId35" display="mailto:parandhama.kokila98@gmail.com"/>
-    <hyperlink ref="F43" r:id="rId36" display="mailto:durgapriyapatnam@gmail.com"/>
-    <hyperlink ref="F44" r:id="rId37" display="mailto:pavannani741@gmail.com"/>
-    <hyperlink ref="F45" r:id="rId38" display="mailto:tejasvimurthy13@gmail.com"/>
-    <hyperlink ref="F46" r:id="rId39" display="mailto:saiprashanthi001@gmail.com"/>
-    <hyperlink ref="F47" r:id="rId40" display="mailto:pragyasharma3007@gmail.com"/>
-    <hyperlink ref="F48" r:id="rId41" display="mailto:r.b.karthik19@gmail.com"/>
-    <hyperlink ref="F49" r:id="rId42" display="mailto:raghavi6anandkumar@gmail.com"/>
-    <hyperlink ref="F50" r:id="rId43" display="mailto:rakshith.kumar.0697@gmail.com"/>
-    <hyperlink ref="F51" r:id="rId44" display="mailto:ram.prashanth97@gmail.com"/>
-    <hyperlink ref="F52" r:id="rId45" display="mailto:lasyaramireddy8@gmail.com"/>
-    <hyperlink ref="F53" r:id="rId46" display="mailto:ranibangale1997@gmail.com"/>
-    <hyperlink ref="F54" r:id="rId47" display="mailto:narainrb97@gmail.com"/>
-    <hyperlink ref="F55" r:id="rId48" display="mailto:mopuriruhia@gmail.com"/>
-    <hyperlink ref="F56" r:id="rId49" display="mailto:vasundhararoyal420@gmail.com"/>
-    <hyperlink ref="F57" r:id="rId50" display="mailto:sj30301@gmail.com"/>
-    <hyperlink ref="F58" r:id="rId51" display="mailto:sahananavale721@gmail.com"/>
-    <hyperlink ref="F59" r:id="rId52" display="mailto:sampadats@gmail.com"/>
-    <hyperlink ref="F60" r:id="rId53" display="mailto:gksandeep97@gmail.com"/>
-    <hyperlink ref="F61" r:id="rId54" display="mailto:kavyasrees143@gmail.com"/>
-    <hyperlink ref="F62" r:id="rId55" display="mailto:shahidafridshaik98@gmail.com"/>
-    <hyperlink ref="F63" r:id="rId56" display="mailto:shivakhilkumar@gmail.com"/>
-    <hyperlink ref="F64" r:id="rId57" display="mailto:shivashankardrif@gmail.com"/>
-    <hyperlink ref="F65" r:id="rId58" display="mailto:sireeshas97@gmail.com"/>
-    <hyperlink ref="F66" r:id="rId59" display="mailto:sirigowda999@gmail.com"/>
-    <hyperlink ref="F67" r:id="rId60" display="mailto:snoubad14@gmail.com"/>
-    <hyperlink ref="F68" r:id="rId61" display="mailto:suralakshmibhavani@gmail.com"/>
-    <hyperlink ref="F69" r:id="rId62" display="mailto:hamsajaanu2000@gmail.com"/>
-    <hyperlink ref="F70" r:id="rId63" display="mailto:premjoshua16@gmail.com"/>
-    <hyperlink ref="F71" r:id="rId64" display="mailto:tramyareddy98@gmail.com"/>
-    <hyperlink ref="F72" r:id="rId65" display="mailto:chaudharyv5221@gmail.com"/>
-    <hyperlink ref="F73" r:id="rId66" display="mailto:varsha9rani@gmail.com"/>
-    <hyperlink ref="F74" r:id="rId67" display="mailto:hadimanividyavat1i@gmail.com"/>
-    <hyperlink ref="F75" r:id="rId68" display="mailto:vindhya.kumbar1@gmail.com"/>
-    <hyperlink ref="F76" r:id="rId69" display="mailto:yasmeendvg97@gmail.com"/>
-    <hyperlink ref="F77" r:id="rId70" display="mailto:srinidhigonal@gmail.com"/>
-    <hyperlink ref="F78" r:id="rId71" display="mailto:divya.ravuri6@gmail.com"/>
-    <hyperlink ref="F79" r:id="rId72" display="mailto:saitejaswinia6@gmail.com"/>
+    <hyperlink ref="L18" r:id="rId1" display="mailto:kalyani.addagada@gmail.com"/>
+    <hyperlink ref="F8" r:id="rId2" display="mailto:amulyaps18@gmail.com"/>
+    <hyperlink ref="F9" r:id="rId3" display="mailto:tanilkumarreddy1998@gmail.com"/>
+    <hyperlink ref="F10" r:id="rId4" display="mailto:anjanashaju1997@gmail.com"/>
+    <hyperlink ref="L22" r:id="rId5" display="mailto:aartipawar070@gmail.com"/>
+    <hyperlink ref="F11" r:id="rId6" display="mailto:akbiswal0108@gmail.com"/>
+    <hyperlink ref="F12" r:id="rId7" display="mailto:hiregoudarpita777@gmail.com"/>
+    <hyperlink ref="F13" r:id="rId8" display="mailto:ashalr1997@gmail.com"/>
+    <hyperlink ref="F14" r:id="rId9" display="mailto:bhavyasree.banyala28@gmail.com"/>
+    <hyperlink ref="L19" r:id="rId10" display="mailto:basavarajtoli1800@gmail.com"/>
+    <hyperlink ref="F15" r:id="rId11" display="mailto:bhagyashree.preety321@gmail.com"/>
+    <hyperlink ref="F16" r:id="rId12" display="mailto:bharathachar437@gmail.com"/>
+    <hyperlink ref="F17" r:id="rId13" display="mailto:bhoomika.n89@gmail.com"/>
+    <hyperlink ref="F18" r:id="rId14" display="mailto:patisagar.1997@gmail.com"/>
+    <hyperlink ref="F19" r:id="rId15" display="mailto:chandulokesh426@gmail.com"/>
+    <hyperlink ref="F20" r:id="rId16" display="mailto:jaggu8191@gmail.com"/>
+    <hyperlink ref="F21" r:id="rId17" display="mailto:tejudesireddy4@gmail.com"/>
+    <hyperlink ref="F22" r:id="rId18" display="mailto:g.pavankalyan1998@gmail.com"/>
+    <hyperlink ref="F23" r:id="rId19" display="mailto:gayathrigayigk18@gmail.com"/>
+    <hyperlink ref="F24" r:id="rId20" display="mailto:yasasvi98@gmail.com"/>
+    <hyperlink ref="F25" r:id="rId21" display="mailto:reshueee.rymec@gmail.com"/>
+    <hyperlink ref="F26" r:id="rId22" display="mailto:kajalsinghmys@gmail.com"/>
+    <hyperlink ref="F27" r:id="rId23" display="mailto:skeerti00@gmail.com"/>
+    <hyperlink ref="F28" r:id="rId24" display="mailto:khadirshaik722@gmail.com"/>
+    <hyperlink ref="F29" r:id="rId25" display="mailto:guna.konda333@gmail.com"/>
+    <hyperlink ref="F30" r:id="rId26" display="mailto:mvmkoushik@gmail.com"/>
+    <hyperlink ref="F31" r:id="rId27" display="mailto:maluguveluanusha@gmail.com"/>
+    <hyperlink ref="F32" r:id="rId28" display="mailto:chundurumahendra@gmail.com"/>
+    <hyperlink ref="F33" r:id="rId29" display="mailto:hussainsaddan786@gmail.com"/>
+    <hyperlink ref="F34" r:id="rId30" display="mailto:vasuda.mikkilineni@gmail.com"/>
+    <hyperlink ref="F35" r:id="rId31" display="mailto:sureshma.reddy1997@gmail.com"/>
+    <hyperlink ref="F36" r:id="rId32" display="mailto:pallavi.nelli1@gmail.com"/>
+    <hyperlink ref="F37" r:id="rId33" display="mailto:mounikasharan4321@gmail.com"/>
+    <hyperlink ref="F38" r:id="rId34" display="mailto:venkatasaiprasad99@gmail.com"/>
+    <hyperlink ref="F39" r:id="rId35" display="mailto:parandhama.kokila98@gmail.com"/>
+    <hyperlink ref="F40" r:id="rId36" display="mailto:durgapriyapatnam@gmail.com"/>
+    <hyperlink ref="F41" r:id="rId37" display="mailto:pavannani741@gmail.com"/>
+    <hyperlink ref="F42" r:id="rId38" display="mailto:tejasvimurthy13@gmail.com"/>
+    <hyperlink ref="F43" r:id="rId39" display="mailto:saiprashanthi001@gmail.com"/>
+    <hyperlink ref="F44" r:id="rId40" display="mailto:pragyasharma3007@gmail.com"/>
+    <hyperlink ref="F45" r:id="rId41" display="mailto:r.b.karthik19@gmail.com"/>
+    <hyperlink ref="F46" r:id="rId42" display="mailto:raghavi6anandkumar@gmail.com"/>
+    <hyperlink ref="F47" r:id="rId43" display="mailto:rakshith.kumar.0697@gmail.com"/>
+    <hyperlink ref="F48" r:id="rId44" display="mailto:ram.prashanth97@gmail.com"/>
+    <hyperlink ref="F49" r:id="rId45" display="mailto:lasyaramireddy8@gmail.com"/>
+    <hyperlink ref="F50" r:id="rId46" display="mailto:ranibangale1997@gmail.com"/>
+    <hyperlink ref="F51" r:id="rId47" display="mailto:narainrb97@gmail.com"/>
+    <hyperlink ref="F52" r:id="rId48" display="mailto:mopuriruhia@gmail.com"/>
+    <hyperlink ref="F53" r:id="rId49" display="mailto:vasundhararoyal420@gmail.com"/>
+    <hyperlink ref="F54" r:id="rId50" display="mailto:sj30301@gmail.com"/>
+    <hyperlink ref="F55" r:id="rId51" display="mailto:sahananavale721@gmail.com"/>
+    <hyperlink ref="F56" r:id="rId52" display="mailto:sampadats@gmail.com"/>
+    <hyperlink ref="L21" r:id="rId53" display="mailto:gksandeep97@gmail.com"/>
+    <hyperlink ref="F57" r:id="rId54" display="mailto:kavyasrees143@gmail.com"/>
+    <hyperlink ref="F58" r:id="rId55" display="mailto:shahidafridshaik98@gmail.com"/>
+    <hyperlink ref="F59" r:id="rId56" display="mailto:shivakhilkumar@gmail.com"/>
+    <hyperlink ref="F60" r:id="rId57" display="mailto:shivashankardrif@gmail.com"/>
+    <hyperlink ref="F61" r:id="rId58" display="mailto:sireeshas97@gmail.com"/>
+    <hyperlink ref="F62" r:id="rId59" display="mailto:sirigowda999@gmail.com"/>
+    <hyperlink ref="F63" r:id="rId60" display="mailto:snoubad14@gmail.com"/>
+    <hyperlink ref="F64" r:id="rId61" display="mailto:suralakshmibhavani@gmail.com"/>
+    <hyperlink ref="F65" r:id="rId62" display="mailto:hamsajaanu2000@gmail.com"/>
+    <hyperlink ref="F66" r:id="rId63" display="mailto:premjoshua16@gmail.com"/>
+    <hyperlink ref="F67" r:id="rId64" display="mailto:tramyareddy98@gmail.com"/>
+    <hyperlink ref="F68" r:id="rId65" display="mailto:chaudharyv5221@gmail.com"/>
+    <hyperlink ref="F69" r:id="rId66" display="mailto:varsha9rani@gmail.com"/>
+    <hyperlink ref="F70" r:id="rId67" display="mailto:hadimanividyavat1i@gmail.com"/>
+    <hyperlink ref="L20" r:id="rId68" display="mailto:vindhya.kumbar1@gmail.com"/>
+    <hyperlink ref="F71" r:id="rId69" display="mailto:yasmeendvg97@gmail.com"/>
+    <hyperlink ref="F72" r:id="rId70" display="mailto:srinidhigonal@gmail.com"/>
+    <hyperlink ref="F73" r:id="rId71" display="mailto:divya.ravuri6@gmail.com"/>
+    <hyperlink ref="F74" r:id="rId72" display="mailto:saitejaswinia6@gmail.com"/>
     <hyperlink ref="L8" r:id="rId73" display="mailto:arpitha.m.dayananda@gmail.com"/>
     <hyperlink ref="L9" r:id="rId74" display="mailto:haripriya4565@gmail.com"/>
     <hyperlink ref="L10" r:id="rId75" display="mailto:harshitamj625@gmail.com"/>
@@ -9341,7 +9335,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L46"/>
+  <dimension ref="B1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9386,7 +9380,7 @@
       </c>
       <c r="D3" s="22">
         <f>COUNT($H$1:$H$100)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="31"/>
     </row>
@@ -9398,7 +9392,7 @@
       </c>
       <c r="D4" s="22">
         <f>COUNT($B$1:$B$100)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="31"/>
     </row>
@@ -9593,6 +9587,21 @@
       <c r="F12" s="17" t="s">
         <v>628</v>
       </c>
+      <c r="H12" s="3">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="5">
+        <v>7743949634</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
@@ -9990,16 +9999,16 @@
         <v>29</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="5">
-        <v>7743949634</v>
+        <v>8624039380</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -10007,16 +10016,16 @@
         <v>30</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E37" s="5">
-        <v>8624039380</v>
+        <v>7218454570</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -10024,16 +10033,16 @@
         <v>31</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E38" s="5">
-        <v>7218454570</v>
+        <v>9359467647</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -10041,16 +10050,16 @@
         <v>32</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E39" s="5">
-        <v>9359467647</v>
+        <v>8691942385</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -10058,16 +10067,16 @@
         <v>33</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E40" s="5">
-        <v>8691942385</v>
+        <v>8850419292</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -10075,16 +10084,16 @@
         <v>34</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E41" s="5">
-        <v>8850419292</v>
+        <v>9621029028</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -10092,16 +10101,16 @@
         <v>35</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E42" s="5">
-        <v>9621029028</v>
+        <v>7066020092</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -10109,16 +10118,16 @@
         <v>36</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E43" s="5">
-        <v>7066020092</v>
+        <v>8349830798</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -10126,16 +10135,16 @@
         <v>37</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E44" s="5">
-        <v>8349830798</v>
+        <v>7225848488</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -10143,32 +10152,15 @@
         <v>38</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E45" s="5">
-        <v>7225848488</v>
+        <v>7719862298</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="3">
-        <v>39</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>695</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="5">
-        <v>7719862298</v>
-      </c>
-      <c r="F46" s="17" t="s">
         <v>696</v>
       </c>
     </row>
@@ -10179,11 +10171,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1"/>
-    <hyperlink ref="F38" r:id="rId2"/>
+    <hyperlink ref="F37" r:id="rId2"/>
     <hyperlink ref="F28" r:id="rId3"/>
     <hyperlink ref="F32" r:id="rId4"/>
     <hyperlink ref="F21" r:id="rId5"/>
-    <hyperlink ref="F39" r:id="rId6"/>
+    <hyperlink ref="F38" r:id="rId6"/>
     <hyperlink ref="F29" r:id="rId7"/>
     <hyperlink ref="F22" r:id="rId8"/>
     <hyperlink ref="F31" r:id="rId9"/>
@@ -10192,20 +10184,20 @@
     <hyperlink ref="F26" r:id="rId12"/>
     <hyperlink ref="F10" r:id="rId13"/>
     <hyperlink ref="F24" r:id="rId14"/>
-    <hyperlink ref="F41" r:id="rId15"/>
+    <hyperlink ref="F40" r:id="rId15"/>
     <hyperlink ref="F13" r:id="rId16"/>
     <hyperlink ref="F35" r:id="rId17"/>
-    <hyperlink ref="F36" r:id="rId18"/>
-    <hyperlink ref="F43" r:id="rId19"/>
-    <hyperlink ref="F44" r:id="rId20"/>
+    <hyperlink ref="L12" r:id="rId18"/>
+    <hyperlink ref="F42" r:id="rId19"/>
+    <hyperlink ref="F43" r:id="rId20"/>
     <hyperlink ref="F23" r:id="rId21"/>
     <hyperlink ref="F14" r:id="rId22"/>
     <hyperlink ref="F12" r:id="rId23"/>
     <hyperlink ref="F25" r:id="rId24"/>
     <hyperlink ref="F11" r:id="rId25"/>
-    <hyperlink ref="F42" r:id="rId26"/>
+    <hyperlink ref="F41" r:id="rId26"/>
     <hyperlink ref="F9" r:id="rId27"/>
-    <hyperlink ref="F37" r:id="rId28"/>
+    <hyperlink ref="F36" r:id="rId28"/>
     <hyperlink ref="F20" r:id="rId29"/>
     <hyperlink ref="F33" r:id="rId30"/>
     <hyperlink ref="F34" r:id="rId31"/>
@@ -10214,9 +10206,9 @@
     <hyperlink ref="F18" r:id="rId34"/>
     <hyperlink ref="F27" r:id="rId35"/>
     <hyperlink ref="F30" r:id="rId36"/>
-    <hyperlink ref="F40" r:id="rId37"/>
-    <hyperlink ref="F45" r:id="rId38"/>
-    <hyperlink ref="F46" r:id="rId39"/>
+    <hyperlink ref="F39" r:id="rId37"/>
+    <hyperlink ref="F44" r:id="rId38"/>
+    <hyperlink ref="F45" r:id="rId39"/>
     <hyperlink ref="L8" r:id="rId40" display="mailto:rukhsarkausar2907@gmail.com"/>
     <hyperlink ref="L9" r:id="rId41" display="mailto:ghadgepratiksha22@gmail.com"/>
     <hyperlink ref="L10" r:id="rId42"/>

</xml_diff>

<commit_message>
Weekly Status Report 17th to 23rd Nov 2019
</commit_message>
<xml_diff>
--- a/HTD Programs-Weekly Status Report for Capgemini.xlsx
+++ b/HTD Programs-Weekly Status Report for Capgemini.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="4" r:id="rId1"/>
@@ -2346,7 +2346,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2465,6 +2465,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4048,7 +4060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4204,11 +4216,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4492,7 +4504,7 @@
       <c r="N6" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="44">
         <v>9897145195</v>
       </c>
       <c r="P6" s="34" t="s">
@@ -4538,14 +4550,14 @@
         <f>'Bangalore Nov Batch Candidates'!D4</f>
         <v>68</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="43" t="s">
         <v>537</v>
       </c>
-      <c r="O7" s="3">
-        <v>9897145195</v>
+      <c r="O7" s="45">
+        <v>8377841525</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>709</v>
@@ -4621,14 +4633,14 @@
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:12" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="H6" s="42" t="s">
+      <c r="C6" s="46"/>
+      <c r="H6" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
@@ -5631,14 +5643,14 @@
       <c r="H5" s="26"/>
     </row>
     <row r="6" spans="2:12" s="19" customFormat="1" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="H6" s="42" t="s">
+      <c r="C6" s="46"/>
+      <c r="H6" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="2:12" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
@@ -5960,14 +5972,14 @@
       <c r="H5" s="26"/>
     </row>
     <row r="6" spans="2:12" s="19" customFormat="1" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="H6" s="42" t="s">
+      <c r="C6" s="46"/>
+      <c r="H6" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="2:12" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
@@ -7527,14 +7539,14 @@
       <c r="H5" s="26"/>
     </row>
     <row r="6" spans="2:12" s="19" customFormat="1" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="H6" s="42" t="s">
+      <c r="C6" s="46"/>
+      <c r="H6" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="2:12" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
@@ -8412,14 +8424,14 @@
       <c r="H5" s="26"/>
     </row>
     <row r="6" spans="2:12" s="19" customFormat="1" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="46" t="s">
         <v>529</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="H6" s="42" t="s">
+      <c r="C6" s="46"/>
+      <c r="H6" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="2:12" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">

</xml_diff>